<commit_message>
Update app.py and requirements.txt for Streamlit Excel fix
</commit_message>
<xml_diff>
--- a/Boiler temps.xlsx
+++ b/Boiler temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vianeyspamers/Documents/whrb_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641A5E66-1DEE-2348-BCD3-F82FDD7A4143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77859350-7229-2342-B368-C8372AECC770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12640" yWindow="500" windowWidth="15780" windowHeight="16080" xr2:uid="{A3A0805D-D9ED-0F42-A628-332E32FF5202}"/>
+    <workbookView xWindow="12640" yWindow="500" windowWidth="15780" windowHeight="16020" xr2:uid="{A3A0805D-D9ED-0F42-A628-332E32FF5202}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B4328D-4335-144F-BCEF-541B54403A17}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -452,6 +452,28 @@
         <v>600</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>3999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>3000</v>
+      </c>
+      <c r="C4">
+        <v>477</v>
+      </c>
+      <c r="D4">
+        <v>633</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>